<commit_message>
Modified UserStories, Acceptance Criteria, added presentation videos
</commit_message>
<xml_diff>
--- a/Xlsx/TestCases.xlsx
+++ b/Xlsx/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemanvithamylapalli/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemanvithamylapalli/Documents/GitHub/2024S-neon-nomads/Xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEF86E9-CE4C-A741-BE1B-14F086ED9D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB79D4E-2988-E24B-B3D8-9F1170F47933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{37383B1C-2FFF-43C8-B959-52A76B07B6D3}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17140" xr2:uid="{37383B1C-2FFF-43C8-B959-52A76B07B6D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Test Id</t>
   </si>
@@ -71,22 +71,9 @@
     <t>USER_ALT_TIME</t>
   </si>
   <si>
-    <t>USER_GEN_REC</t>
-  </si>
-  <si>
-    <t>USER_FIL_PREF</t>
-  </si>
-  <si>
-    <t>USER_INSUFF_ERR</t>
-  </si>
-  <si>
     <t>Time frames for when the alerts should be sent.</t>
   </si>
   <si>
-    <t>System’s response when there are insufficient items
- for any recipe recommendation.</t>
-  </si>
-  <si>
     <t>USER_SGN</t>
   </si>
   <si>
@@ -121,15 +108,6 @@
   </si>
   <si>
     <t>Successfully setting Time frames for alerts</t>
-  </si>
-  <si>
-    <t>Successful recipe recommendation genration</t>
-  </si>
-  <si>
-    <t>Successful recipe filtering</t>
-  </si>
-  <si>
-    <t>User Insufficient items for recipe error</t>
   </si>
   <si>
     <t>Verify sign-up process with valid data.</t>
@@ -160,12 +138,13 @@
 expiry dates.</t>
   </si>
   <si>
-    <t>Test generating recipe recommendations based on current 
-pantry items.</t>
-  </si>
-  <si>
-    <t>Test Filtering recipes based on dietary restrictions or 
-preferences.</t>
+    <t>Test recipe recogniser  when you upload an image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successful recipe recogniser </t>
+  </si>
+  <si>
+    <t>USER_REC</t>
   </si>
 </sst>
 </file>
@@ -181,10 +160,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,7 +189,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -550,13 +529,13 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="41.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -564,7 +543,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -573,90 +552,90 @@
     </row>
     <row r="2" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>33</v>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>34</v>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>35</v>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>36</v>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>37</v>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>38</v>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -664,55 +643,39 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>